<commit_message>
Arregle algunos errores debido a inconsistencias en archivos excel.
</commit_message>
<xml_diff>
--- a/testData/datosAdicionales.xlsx
+++ b/testData/datosAdicionales.xlsx
@@ -131,7 +131,7 @@
     <t xml:space="preserve">Electricidad y magnetismo</t>
   </si>
   <si>
-    <t xml:space="preserve">Instalaciones Eléctricas</t>
+    <t xml:space="preserve">Instalaciones eléctricas</t>
   </si>
   <si>
     <t xml:space="preserve">Control de calidad</t>
@@ -150,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -183,6 +183,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -228,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,12 +248,16 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -269,10 +280,10 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -642,276 +653,255 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>